<commit_message>
Changes proposed by David Tao implemented
</commit_message>
<xml_diff>
--- a/documents/Peer Review Comments/2014_03_vMR_LM_peer_review/vMR Logical Model Change Log based on 2014-03 peer review.xlsx
+++ b/documents/Peer Review Comments/2014_03_vMR_LM_peer_review/vMR Logical Model Change Log based on 2014-03 peer review.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Pending</t>
   </si>
   <si>
     <t>Section 2.  Daft Standard --&gt; Draft Standard</t>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>p. 27, Patient Problems, etc.: Patient diagnoses and traits --&gt; Patient problems</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -142,6 +142,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -189,7 +192,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,7 +227,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,7 +439,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +468,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -473,10 +476,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -484,10 +487,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -495,10 +498,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -506,10 +509,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -517,10 +520,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,10 +531,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -539,10 +542,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -550,10 +553,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>